<commit_message>
Empezando segundo semestre de 2do ano
</commit_message>
<xml_diff>
--- a/2do año/Sexto Semestre/horarios.xlsx
+++ b/2do año/Sexto Semestre/horarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\importante\Facultad\2do año\Sexto Semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Facultad\2do año\Sexto Semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B52C27-5F4D-4043-B5AC-DA4335CA437B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D528EC5-CBF7-4523-AD57-087EE10FC744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t>Lunes</t>
   </si>
@@ -71,12 +71,6 @@
     <t>OO1</t>
   </si>
   <si>
-    <t>FALTA VER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMISION </t>
-  </si>
-  <si>
     <t>INGE1</t>
   </si>
   <si>
@@ -86,12 +80,6 @@
     <t xml:space="preserve">AULA 14 </t>
   </si>
   <si>
-    <t>SI VAMOS A</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t xml:space="preserve"> AULA 5</t>
   </si>
   <si>
@@ -102,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>exPRACTICA</t>
   </si>
 </sst>
 </file>
@@ -169,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -264,17 +255,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -365,73 +345,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,26 +418,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,12 +776,12 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -821,166 +799,166 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="26" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.35416666666666669</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="37" t="s">
+      <c r="D3" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="30"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.375</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.39583333333333298</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="31" t="s">
+      <c r="D5" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0.41666666666666702</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="31" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="43"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="42"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0.4375</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="48" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="31"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="48" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="32"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="F8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
         <v>0.5</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="29" t="s">
+      <c r="E10" s="22"/>
+      <c r="F10" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="29" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="32"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="1"/>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>0.5625</v>
       </c>
@@ -988,7 +966,7 @@
       <c r="C13" s="10"/>
       <c r="D13" s="1"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="26" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -998,221 +976,212 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>0.58333333333333304</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="28" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="27" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="K14" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>0.60416666666666696</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15" s="23"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="28" t="s">
+      <c r="E15" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="27" t="s">
         <v>7</v>
       </c>
+      <c r="H15" s="48"/>
       <c r="I15" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>0.625</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="22" t="s">
+        <v>7</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="I16" s="4"/>
-      <c r="K16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>0.64583333333333404</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="23" t="s">
-        <v>6</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="35"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="I18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>0.6875</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="23"/>
+      <c r="B19" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="34"/>
       <c r="D19" s="9"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="I19" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="I19" s="3"/>
       <c r="K19" s="6"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="33"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="I20" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="I20" s="3"/>
       <c r="K20" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B21" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="34" t="s">
-        <v>14</v>
+      <c r="B21" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="I21" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="I21" s="3"/>
       <c r="K21" s="6"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
         <v>0.75</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
         <v>0.75</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="18"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>8</v>
+      <c r="B24" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="20" t="s">
-        <v>14</v>
+      <c r="D24" s="20"/>
+      <c r="E24" s="19" t="s">
+        <v>12</v>
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="15">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="19" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
         <v>0.812500000000001</v>
       </c>
-      <c r="B26" s="24"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="20" t="s">
-        <v>15</v>
+      <c r="E26" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>0.83333333333333404</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="1"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="21"/>
+      <c r="E27" s="20"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>0.85416666666666696</v>
       </c>
@@ -1222,7 +1191,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>0.875000000000001</v>
       </c>

</xml_diff>

<commit_message>
agregando cosas iso, dbd, inge1
</commit_message>
<xml_diff>
--- a/2do año/Sexto Semestre/horarios.xlsx
+++ b/2do año/Sexto Semestre/horarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Facultad\2do año\Sexto Semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\importante\Facultad\2do año\Sexto Semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D528EC5-CBF7-4523-AD57-087EE10FC744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2053E63-1A4A-473C-81EF-4E98244A3015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
+    <workbookView xWindow="3960" yWindow="2925" windowWidth="20910" windowHeight="11835" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -414,7 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,17 +427,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,12 +776,12 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -799,19 +799,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="39"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="26" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.35416666666666669</v>
       </c>
@@ -819,7 +819,7 @@
       <c r="C3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="36" t="s">
@@ -827,7 +827,7 @@
       </c>
       <c r="F3" s="29"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.375</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="C4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="36" t="s">
@@ -845,7 +845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.39583333333333298</v>
       </c>
@@ -853,7 +853,7 @@
       <c r="C5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="37"/>
@@ -861,54 +861,54 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0.41666666666666702</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="37"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="46"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="42"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.4375</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="47" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="46" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="30"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="47" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="46" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="22" t="s">
         <v>7</v>
       </c>
@@ -916,11 +916,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>0.5</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="30" t="s">
@@ -932,11 +932,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="39" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="30" t="s">
@@ -948,17 +948,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="41"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="31"/>
       <c r="D12" s="1"/>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>0.5625</v>
       </c>
@@ -976,7 +976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>0.58333333333333304</v>
       </c>
@@ -992,7 +992,7 @@
       <c r="I14" s="4"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>0.60416666666666696</v>
       </c>
@@ -1005,7 +1005,6 @@
       <c r="F15" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="48"/>
       <c r="I15" s="4" t="s">
         <v>17</v>
       </c>
@@ -1013,7 +1012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>0.625</v>
       </c>
@@ -1027,7 +1026,7 @@
       <c r="I16" s="4"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>0.64583333333333404</v>
       </c>
@@ -1037,7 +1036,7 @@
       <c r="E17" s="23"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>0.66666666666666696</v>
       </c>
@@ -1056,7 +1055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>0.6875</v>
       </c>
@@ -1071,7 +1070,7 @@
       <c r="K19" s="6"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>0.70833333333333404</v>
       </c>
@@ -1088,7 +1087,7 @@
       </c>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>0.72916666666666696</v>
       </c>
@@ -1105,7 +1104,7 @@
       <c r="K21" s="6"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>0.75</v>
       </c>
@@ -1117,7 +1116,7 @@
       <c r="E22" s="17"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>0.75</v>
       </c>
@@ -1131,7 +1130,7 @@
       <c r="E23" s="18"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>0.77083333333333404</v>
       </c>
@@ -1145,7 +1144,7 @@
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>0.79166666666666696</v>
       </c>
@@ -1159,7 +1158,7 @@
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>0.812500000000001</v>
       </c>
@@ -1171,7 +1170,7 @@
       </c>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>0.83333333333333404</v>
       </c>
@@ -1181,7 +1180,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>0.85416666666666696</v>
       </c>
@@ -1191,7 +1190,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>0.875000000000001</v>
       </c>

</xml_diff>

<commit_message>
iso e oo1 apuntes
</commit_message>
<xml_diff>
--- a/2do año/Sexto Semestre/horarios.xlsx
+++ b/2do año/Sexto Semestre/horarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\importante\Facultad\2do año\Sexto Semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Facultad\2do año\Sexto Semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2053E63-1A4A-473C-81EF-4E98244A3015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7C90AA-2D7D-4325-B27A-C4E9D6C42A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2925" windowWidth="20910" windowHeight="11835" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -339,9 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -776,12 +773,12 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -799,174 +796,180 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.35416666666666669</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.375</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.39583333333333298</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0.41666666666666702</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="30" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="41"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="40"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0.4375</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="46" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="30"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="F7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="46" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="31"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
         <v>0.5</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="21"/>
+      <c r="F10" s="27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="28" t="s">
+      <c r="E11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="31"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="21" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>0.5625</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="10"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="26" t="s">
+      <c r="E13" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -976,33 +979,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>0.58333333333333304</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="27" t="s">
+      <c r="E14" s="22"/>
+      <c r="F14" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="4"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>0.60416666666666696</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="1"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="27" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="26" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -1012,37 +1011,35 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>0.625</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="22" t="s">
-        <v>7</v>
-      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="11"/>
       <c r="I16" s="4"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>0.64583333333333404</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="1"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="34"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="I18" s="3" t="s">
@@ -1055,14 +1052,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
         <v>0.6875</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="9"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1070,15 +1067,15 @@
       <c r="K19" s="6"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="32"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="I20" s="3"/>
@@ -1087,15 +1084,15 @@
       </c>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="33" t="s">
+      <c r="C21" s="33"/>
+      <c r="D21" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="1"/>
@@ -1104,83 +1101,83 @@
       <c r="K21" s="6"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
         <v>0.75</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
         <v>0.75</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="19" t="s">
+      <c r="D24" s="19"/>
+      <c r="E24" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
         <v>0.812500000000001</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="18" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>0.83333333333333404</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="1"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="20"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>0.85416666666666696</v>
       </c>
@@ -1190,7 +1187,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>0.875000000000001</v>
       </c>

</xml_diff>

<commit_message>
arreglando horarios y haciendo historias de usuario de inge1
</commit_message>
<xml_diff>
--- a/2do año/Sexto Semestre/horarios.xlsx
+++ b/2do año/Sexto Semestre/horarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\importante\Facultad\2do año\Sexto Semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2053E63-1A4A-473C-81EF-4E98244A3015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7773712E-01C6-4806-A235-ED4A5746C4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2925" windowWidth="20910" windowHeight="11835" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
+    <workbookView xWindow="3960" yWindow="780" windowWidth="20910" windowHeight="13980" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>Lunes</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>exPRACTICA</t>
   </si>
 </sst>
 </file>
@@ -301,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -339,9 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -776,7 +770,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,43 +799,43 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.35416666666666669</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.375</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="29" t="s">
         <v>9</v>
       </c>
     </row>
@@ -850,14 +844,14 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="29" t="s">
         <v>6</v>
       </c>
     </row>
@@ -866,96 +860,98 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="30" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="41"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.4375</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="46" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="30"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="46" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="31"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>0.5</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="21"/>
+      <c r="F10" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="28" t="s">
+      <c r="E11" s="22"/>
+      <c r="F11" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="14">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="31"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -965,8 +961,10 @@
       <c r="B13" s="12"/>
       <c r="C13" s="10"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="26" t="s">
+      <c r="E13" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -984,9 +982,9 @@
       <c r="C14" s="8"/>
       <c r="D14" s="1"/>
       <c r="E14" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="4"/>
@@ -999,10 +997,8 @@
       <c r="B15" s="8"/>
       <c r="C15" s="1"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="27" t="s">
+      <c r="E15" s="22"/>
+      <c r="F15" s="26" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -1018,10 +1014,8 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="22" t="s">
-        <v>7</v>
-      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="11"/>
       <c r="I16" s="4"/>
       <c r="K16" s="5"/>
@@ -1033,16 +1027,16 @@
       <c r="B17" s="8"/>
       <c r="C17" s="1"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="34"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="I18" s="3" t="s">
@@ -1056,13 +1050,13 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19" s="14">
         <v>0.6875</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="9"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1071,14 +1065,14 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="A20" s="14">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="32"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="I20" s="3"/>
@@ -1088,14 +1082,14 @@
       <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="A21" s="14">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="33" t="s">
+      <c r="C21" s="33"/>
+      <c r="D21" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="1"/>
@@ -1105,67 +1099,61 @@
       <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="A22" s="14">
         <v>0.75</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="A23" s="14">
         <v>0.75</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>10</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="14">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>18</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="19" t="s">
+      <c r="D24" s="19"/>
+      <c r="E24" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="A25" s="14">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B25" s="22" t="s">
-        <v>7</v>
-      </c>
+      <c r="B25" s="1"/>
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26" s="14">
         <v>0.812500000000001</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="1"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="18" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="9"/>
@@ -1177,7 +1165,7 @@
       <c r="B27" s="12"/>
       <c r="C27" s="1"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="20"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Haciendo ej3,4,5 de OO1
</commit_message>
<xml_diff>
--- a/2do año/Sexto Semestre/horarios.xlsx
+++ b/2do año/Sexto Semestre/horarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\importante\Facultad\2do año\Sexto Semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8138EC-9147-4493-B140-6C80DEF22E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7456C03-BED3-491F-A3FD-5A8F40E8CFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="780" windowWidth="20910" windowHeight="13980" xr2:uid="{28D87BDB-8089-4128-B228-EC0F311DB0A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>Lunes</t>
   </si>
@@ -74,16 +74,7 @@
     <t>INGE1</t>
   </si>
   <si>
-    <t>AYED RED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AULA 14 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> AULA 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AULA 8 </t>
   </si>
   <si>
     <t xml:space="preserve"> AULA 4</t>
@@ -113,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,12 +137,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -298,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,9 +303,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,18 +327,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -366,12 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -388,12 +355,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -767,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C9F149-6F44-46BF-BA0A-FA8F2E963F98}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +747,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -798,44 +759,44 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="25" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.375</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
     </row>
@@ -843,15 +804,15 @@
       <c r="A5" s="2">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="29" t="s">
+      <c r="D5" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="23" t="s">
         <v>6</v>
       </c>
     </row>
@@ -859,112 +820,112 @@
       <c r="A6" s="2">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="29" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="40"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.4375</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="45" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="45" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="30"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>0.5</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="27" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="27" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>0.5625</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="19" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -978,13 +939,13 @@
       <c r="A14" s="2">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="4"/>
@@ -994,49 +955,49 @@
       <c r="A15" s="2">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="26" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="20" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>0.625</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="33"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="10"/>
       <c r="I16" s="4"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>0.64583333333333404</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="33"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="I18" s="3" t="s">
@@ -1045,140 +1006,116 @@
       <c r="K18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>0.6875</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="9"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="I19" s="3"/>
       <c r="K19" s="6"/>
-      <c r="M19" s="7"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="31"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="I20" s="3"/>
       <c r="K20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M20" s="7"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="32" t="s">
-        <v>12</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="I21" s="3"/>
       <c r="K21" s="6"/>
-      <c r="M21" s="7"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <v>0.75</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="16"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
         <v>0.75</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
+      <c r="C23" s="8"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>0.77083333333333404</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
+      <c r="C24" s="8"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
         <v>0.79166666666666696</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+      <c r="C25" s="8"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
         <v>0.812500000000001</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C26" s="8"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>0.83333333333333404</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="7"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>0.85416666666666696</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="12"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>0.875000000000001</v>
       </c>

</xml_diff>